<commit_message>
Added Myers Briggs table
</commit_message>
<xml_diff>
--- a/Documents/Profile Data.xlsx
+++ b/Documents/Profile Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natal\Documents\GitHub\syntechnologies.github.io\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9A2E4C2-4F6A-4B19-A631-0D48C07C5818}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CBA3CF-E35E-470D-9ED8-D18687D2ABE7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15285" yWindow="630" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{5F0727B8-A82A-41B9-9188-7B0F38E3A1DC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5F0727B8-A82A-41B9-9188-7B0F38E3A1DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>Natalie Yelland-Hall</t>
   </si>
@@ -97,6 +97,93 @@
   <si>
     <t>Myers Brigs</t>
   </si>
+  <si>
+    <t>Mind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy </t>
+  </si>
+  <si>
+    <t>Nature</t>
+  </si>
+  <si>
+    <t>Tactics</t>
+  </si>
+  <si>
+    <t>Identity</t>
+  </si>
+  <si>
+    <t>88% Extraverted</t>
+  </si>
+  <si>
+    <t>64% Intuituve</t>
+  </si>
+  <si>
+    <t>51% Feeling</t>
+  </si>
+  <si>
+    <t>51% Prospecting</t>
+  </si>
+  <si>
+    <t>53% Assertive</t>
+  </si>
+  <si>
+    <t>100% Introverted</t>
+  </si>
+  <si>
+    <t>63% Observant</t>
+  </si>
+  <si>
+    <t>60% Feeling</t>
+  </si>
+  <si>
+    <t>71% Judging</t>
+  </si>
+  <si>
+    <t>65% Turbulent</t>
+  </si>
+  <si>
+    <t>57% Extroverted</t>
+  </si>
+  <si>
+    <t>68% Observant</t>
+  </si>
+  <si>
+    <t>56% Prospecting</t>
+  </si>
+  <si>
+    <t>56%Assertive</t>
+  </si>
+  <si>
+    <t>79% Introverted</t>
+  </si>
+  <si>
+    <t>56% Observant</t>
+  </si>
+  <si>
+    <t>68% Thinking</t>
+  </si>
+  <si>
+    <t>64% Prospecting</t>
+  </si>
+  <si>
+    <t>97% Turbulent</t>
+  </si>
+  <si>
+    <t>65% Introverted</t>
+  </si>
+  <si>
+    <t>56% Feeling</t>
+  </si>
+  <si>
+    <t>75% Judging</t>
+  </si>
+  <si>
+    <t>76% Assertive</t>
+  </si>
+  <si>
+    <t>Names</t>
+  </si>
 </sst>
 </file>
 
@@ -156,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -164,11 +251,103 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -5904,6 +6083,30 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83CB8BD6-D722-4601-967D-57C93016C73A}" name="Table1" displayName="Table1" ref="A1:G7" headerRowDxfId="2">
+  <autoFilter ref="A1:G7" xr:uid="{3922BB13-C4EA-4BF1-A41B-6FE1652D756D}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{F37EB24A-856D-4C8B-833B-012D0D548634}" name="Names" totalsRowLabel="Total" dataDxfId="4" totalsRowDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{F3428BCB-CCDF-4401-8E6D-4AA60B6A0160}" name="Myers Brigs" dataDxfId="3" totalsRowDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{4039A8DB-B801-4DA2-8DE2-0074BDE68338}" name="Mind"/>
+    <tableColumn id="4" xr3:uid="{6383184B-88CC-4D90-880A-16A610D77079}" name="Energy "/>
+    <tableColumn id="5" xr3:uid="{C7C587BF-B6E7-40F4-ACB4-649F4036CED6}" name="Nature"/>
+    <tableColumn id="6" xr3:uid="{617F0149-7BE6-41B9-862D-69F1F779CBEE}" name="Tactics"/>
+    <tableColumn id="7" xr3:uid="{311432EF-00F2-41AA-909C-A018526D0CE4}" name="Identity" totalsRowFunction="count"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6203,24 +6406,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45505262-B2A5-42F8-97BA-84DCC40A07B9}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="A1:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -6228,51 +6454,129 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -6441,7 +6745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F83E438-0EAB-40DC-B2D5-A9A1B961F7E6}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Jae to myers briggs table
</commit_message>
<xml_diff>
--- a/Documents/Profile Data.xlsx
+++ b/Documents/Profile Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natal\Documents\GitHub\syntechnologies.github.io\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CBA3CF-E35E-470D-9ED8-D18687D2ABE7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0212320-246E-4C3F-A714-9101C4320B0E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5F0727B8-A82A-41B9-9188-7B0F38E3A1DC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
   <si>
     <t>Natalie Yelland-Hall</t>
   </si>
@@ -184,6 +184,21 @@
   <si>
     <t>Names</t>
   </si>
+  <si>
+    <t>78% Introverted</t>
+  </si>
+  <si>
+    <t>77% Intuitive</t>
+  </si>
+  <si>
+    <t>58% Feeling</t>
+  </si>
+  <si>
+    <t>76% Judging</t>
+  </si>
+  <si>
+    <t>63% Turbulent</t>
+  </si>
 </sst>
 </file>
 
@@ -259,7 +274,7 @@
   <dxfs count="5">
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -313,7 +328,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -6086,7 +6101,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83CB8BD6-D722-4601-967D-57C93016C73A}" name="Table1" displayName="Table1" ref="A1:G7" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83CB8BD6-D722-4601-967D-57C93016C73A}" name="Table1" displayName="Table1" ref="A1:G7" headerRowDxfId="4">
   <autoFilter ref="A1:G7" xr:uid="{3922BB13-C4EA-4BF1-A41B-6FE1652D756D}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -6097,8 +6112,8 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F37EB24A-856D-4C8B-833B-012D0D548634}" name="Names" totalsRowLabel="Total" dataDxfId="4" totalsRowDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{F3428BCB-CCDF-4401-8E6D-4AA60B6A0160}" name="Myers Brigs" dataDxfId="3" totalsRowDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{F37EB24A-856D-4C8B-833B-012D0D548634}" name="Names" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{F3428BCB-CCDF-4401-8E6D-4AA60B6A0160}" name="Myers Brigs" dataDxfId="1" totalsRowDxfId="0"/>
     <tableColumn id="3" xr3:uid="{4039A8DB-B801-4DA2-8DE2-0074BDE68338}" name="Mind"/>
     <tableColumn id="4" xr3:uid="{6383184B-88CC-4D90-880A-16A610D77079}" name="Energy "/>
     <tableColumn id="5" xr3:uid="{C7C587BF-B6E7-40F4-ACB4-649F4036CED6}" name="Nature"/>
@@ -6453,6 +6468,21 @@
       <c r="B2" t="s">
         <v>14</v>
       </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">

</xml_diff>